<commit_message>
BMS and BLE Merged to source
</commit_message>
<xml_diff>
--- a/rpm2pwm/Book1.xlsx
+++ b/rpm2pwm/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/kjung03_student_ubc_ca/Documents/Documents/ELEC391/ELEC391_SteadyCart/rpm2pwm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="8_{E3E0A1C6-B070-4C6C-AB77-F82FCFDC7161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83429B8F-B061-4D2C-BB27-4D4F4BA39ADC}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{E3E0A1C6-B070-4C6C-AB77-F82FCFDC7161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C83C1572-6673-4BA1-92B7-E6B436A2C465}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{50C772FE-0D89-42DE-8FFB-535531E959F5}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>rpm</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>3rd</t>
+  </si>
+  <si>
+    <t>pow</t>
   </si>
 </sst>
 </file>
@@ -233,43 +236,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="65000"/>
-                            <a:lumOff val="35000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>y = 0.000675698364746x</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="30000"/>
-                      <a:t>2.079153042372970</a:t>
-                    </a:r>
-                    <a:br>
-                      <a:rPr lang="en-US" baseline="0"/>
-                    </a:br>
-                    <a:r>
-                      <a:rPr lang="en-US" baseline="0"/>
-                      <a:t>R² = 0.88449042449904</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
               <c:numFmt formatCode="#,##0.000000000000000" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1166,6 +1132,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7EB9E2BF-27F9-4F25-872E-9F359AEEFA9D}" name="Table1" displayName="Table1" ref="A1:B11" tableType="xml" totalsRowShown="0" connectionId="1">
   <autoFilter ref="A1:B11" xr:uid="{7EB9E2BF-27F9-4F25-872E-9F359AEEFA9D}"/>
@@ -1496,10 +1466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1508,7 +1478,7 @@
     <col min="2" max="2" width="6.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1519,10 +1489,13 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>210</v>
       </c>
@@ -1537,8 +1510,12 @@
         <f>0.000675698364746*POWER(Table1[[#This Row],[rpm]],2.07915394237297)</f>
         <v>45.499253320580237</v>
       </c>
+      <c r="G2">
+        <f>11.1699046314716*EXP(0.006864839435544*Table1[[#This Row],[rpm]])</f>
+        <v>47.221030584673869</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>300</v>
       </c>
@@ -1553,8 +1530,12 @@
         <f>0.000675698364746*POWER(Table1[[#This Row],[rpm]],2.07915394237297)</f>
         <v>95.514496437250941</v>
       </c>
+      <c r="G3">
+        <f>11.1699046314716*EXP(0.006864839435544*Table1[[#This Row],[rpm]])</f>
+        <v>87.590706820540589</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>349.2</v>
       </c>
@@ -1569,8 +1550,12 @@
         <f>0.000675698364746*POWER(Table1[[#This Row],[rpm]],2.07915394237297)</f>
         <v>130.97719621919484</v>
       </c>
+      <c r="G4">
+        <f>11.1699046314716*EXP(0.006864839435544*Table1[[#This Row],[rpm]])</f>
+        <v>122.78379027964148</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>375.96</v>
       </c>
@@ -1585,8 +1570,12 @@
         <f>0.000675698364746*POWER(Table1[[#This Row],[rpm]],2.07915394237297)</f>
         <v>152.71045206997704</v>
       </c>
+      <c r="G5">
+        <f>11.1699046314716*EXP(0.006864839435544*Table1[[#This Row],[rpm]])</f>
+        <v>147.54424683168094</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>394.8</v>
       </c>
@@ -1601,8 +1590,12 @@
         <f>0.000675698364746*POWER(Table1[[#This Row],[rpm]],2.07915394237297)</f>
         <v>169.05212829562242</v>
       </c>
+      <c r="G6">
+        <f>11.1699046314716*EXP(0.006864839435544*Table1[[#This Row],[rpm]])</f>
+        <v>167.91563560911743</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>406.8</v>
       </c>
@@ -1617,8 +1610,12 @@
         <f>0.000675698364746*POWER(Table1[[#This Row],[rpm]],2.07915394237297)</f>
         <v>179.91092865585088</v>
       </c>
+      <c r="G7">
+        <f>11.1699046314716*EXP(0.006864839435544*Table1[[#This Row],[rpm]])</f>
+        <v>182.33392477867912</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>416.4</v>
       </c>
@@ -1633,8 +1630,12 @@
         <f>0.000675698364746*POWER(Table1[[#This Row],[rpm]],2.07915394237297)</f>
         <v>188.85083535674704</v>
       </c>
+      <c r="G8">
+        <f>11.1699046314716*EXP(0.006864839435544*Table1[[#This Row],[rpm]])</f>
+        <v>194.75497229149673</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>423</v>
       </c>
@@ -1649,8 +1650,12 @@
         <f>0.000675698364746*POWER(Table1[[#This Row],[rpm]],2.07915394237297)</f>
         <v>195.12764215228705</v>
       </c>
+      <c r="G9">
+        <f>11.1699046314716*EXP(0.006864839435544*Table1[[#This Row],[rpm]])</f>
+        <v>203.78186985657427</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>435</v>
       </c>
@@ -1665,8 +1670,12 @@
         <f>0.000675698364746*POWER(Table1[[#This Row],[rpm]],2.07915394237297)</f>
         <v>206.81317806449778</v>
       </c>
+      <c r="G10">
+        <f>11.1699046314716*EXP(0.006864839435544*Table1[[#This Row],[rpm]])</f>
+        <v>221.27985875110303</v>
+      </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>120</v>
       </c>
@@ -1677,6 +1686,10 @@
       <c r="F11">
         <f>0.000675698364746*POWER(Table1[[#This Row],[rpm]],2.07915394237297)</f>
         <v>14.213163519069322</v>
+      </c>
+      <c r="G11">
+        <f>11.1699046314716*EXP(0.006864839435544*Table1[[#This Row],[rpm]])</f>
+        <v>25.457332294934702</v>
       </c>
     </row>
   </sheetData>

</xml_diff>